<commit_message>
Change title header excel
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_purchase/static/src/xlsx/template_po_noi_dia_ver2.0.xlsx
+++ b/addons/custom/forlife_purchase/static/src/xlsx/template_po_noi_dia_ver2.0.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Forlife\code\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aht\Desktop\Forlife\m_onnet_odoo_mfl2201er\addons\custom\forlife_purchase\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60663DAB-3207-40CB-852A-DB8E0AD36BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PO - HH" sheetId="2" r:id="rId1"/>
@@ -22,13 +21,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>DELL</author>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{38A201AB-FA9F-4A2C-857F-883CF758D73A}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="1" shapeId="0" xr:uid="{56C6A7C2-98CB-45BE-99CC-C0709C07AD5F}">
+    <comment ref="K1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{FFCD09BB-7986-4C81-ACAE-594C66B213F2}">
+    <comment ref="L1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="1" shapeId="0" xr:uid="{202938D7-88EA-4A28-BAC5-37D9B2AE089A}">
+    <comment ref="O1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{CAF63FE3-42F4-42D4-B00B-F5329739AD82}">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -141,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{43E851DA-1E7D-4B7B-86F6-F620CE653CC0}">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -168,13 +167,13 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
     <author>DELL</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{3E7DBBB6-6DA6-43F9-BB77-319144B7DFB2}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{B3441D31-85C4-4ADE-BED0-372B79909630}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{23B017A6-16A1-47E0-8B43-CB09FE54DB50}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -248,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="1" shapeId="0" xr:uid="{237ADBD6-10BD-45A5-8520-6D61B6CC87EF}">
+    <comment ref="V1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +269,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="1" shapeId="0" xr:uid="{FFC5AAA4-7B47-4500-8129-FECCCE9382F1}">
+    <comment ref="W1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -297,12 +296,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Văn Quyết (DU01 PTPM)</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{2CF4CA4D-C97D-4881-A863-B3C3F5E9D7FC}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -326,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{B0289F6E-FFDC-429D-B65D-6245DFD5729F}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{45C6E384-E8BF-49A4-9DBB-3E9EE9EE607F}">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -381,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="66">
   <si>
     <t>Note</t>
   </si>
@@ -625,7 +624,7 @@
   </si>
   <si>
     <r>
-      <t>Chi tiết đơn hàng / Số lượng quy đổi (</t>
+      <t>Chi tiết đơn hàng / Địa điểm kho (</t>
     </r>
     <r>
       <rPr>
@@ -650,7 +649,7 @@
   </si>
   <si>
     <r>
-      <t>Chi tiết đơn hàng / Địa điểm kho (</t>
+      <t>Chi tiết đơn hàng / Ngày nhận (</t>
     </r>
     <r>
       <rPr>
@@ -674,8 +673,14 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Chi tiết đơn hàng / Ngày nhận (</t>
+    <t>Chi tiết đơn hàng / STT Dòng YCMH</t>
+  </si>
+  <si>
+    <t>Chi phí / Mã Sản phẩm</t>
+  </si>
+  <si>
+    <r>
+      <t>Tiền tệ (</t>
     </r>
     <r>
       <rPr>
@@ -693,20 +698,15 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
-    <t>Chi tiết đơn hàng / STT Dòng YCMH</t>
-  </si>
-  <si>
-    <t>Chi phí / Mã Sản phẩm</t>
-  </si>
-  <si>
-    <r>
-      <t>Tiền tệ (</t>
+    <r>
+      <t>Tỷ giá (</t>
     </r>
     <r>
       <rPr>
@@ -724,18 +724,231 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Hạn xử lý  (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>)</t>
     </r>
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Chi tiết đơn hàng / Đơn vị mua </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Giá của nhà cung cấp (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / Thành tiền VND của sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / % Thuế nhập khẩu</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / Thuế nhập khẩu của sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / % Thuế tiêu thụ đặc biệt</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  /  Thuế TTĐB của sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / % Thuế GTGT</t>
+  </si>
+  <si>
+    <t>Chi tiết đơn hàng  / Thuế GTGT của sản phẩm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chi phí / Tiền tệ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>Nhập khẩu quần áo</t>
+  </si>
+  <si>
+    <t>1551_TP001</t>
+  </si>
+  <si>
+    <t>POLO2023</t>
+  </si>
+  <si>
+    <t>PR204</t>
+  </si>
+  <si>
+    <t>1562_CPHH</t>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Số lượng (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chi tiết đơn hàng / Đơn giá </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>622_NCNB</t>
+  </si>
+  <si>
+    <r>
       <t>Tỷ giá (</t>
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
@@ -757,7 +970,7 @@
   </si>
   <si>
     <r>
-      <t>Hạn xử lý  (</t>
+      <t>Kho nhận (</t>
     </r>
     <r>
       <rPr>
@@ -765,6 +978,54 @@
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Địa điểm xuất NPL</t>
+  </si>
+  <si>
+    <t>1000000041</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Mã Sản phẩm</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tiền tệ</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tỷ giá</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Tổng tiền ngoại tệ̣</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Thành tiền VND</t>
+  </si>
+  <si>
+    <t>Chi phí ước tính / Chi phí trước thuế</t>
+  </si>
+  <si>
+    <r>
+      <t>Chi tiết đơn hàng / Tỷ lệ quy đổi (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
       </rPr>
@@ -779,259 +1040,12 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chi tiết đơn hàng / Đơn vị mua </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Chi tiết đơn hàng / Giá của nhà cung cấp (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / Thành tiền VND của sản phẩm</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / % Thuế nhập khẩu</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / Thuế nhập khẩu của sản phẩm</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / % Thuế tiêu thụ đặc biệt</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  /  Thuế TTĐB của sản phẩm</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / % Thuế GTGT</t>
-  </si>
-  <si>
-    <t>Chi tiết đơn hàng  / Thuế GTGT của sản phẩm</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chi phí / Tiền tệ </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>Nhập khẩu quần áo</t>
-  </si>
-  <si>
-    <t>1551_TP001</t>
-  </si>
-  <si>
-    <t>POLO2023</t>
-  </si>
-  <si>
-    <t>PR204</t>
-  </si>
-  <si>
-    <t>1562_CPHH</t>
-  </si>
-  <si>
-    <r>
-      <t>Chi tiết đơn hàng / Số lượng (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Chi tiết đơn hàng / Đơn giá </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>622_NCNB</t>
-  </si>
-  <si>
-    <r>
-      <t>Tỷ giá (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="163"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Kho nhận (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Địa điểm xuất NPL</t>
-  </si>
-  <si>
-    <t>Chi phí / Tiền tệ</t>
-  </si>
-  <si>
-    <t>1000000041</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-1010000]d/m/yyyy;@"/>
@@ -1241,37 +1255,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1611,11 +1595,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y27" sqref="Y27"/>
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1670,10 +1654,10 @@
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>23</v>
@@ -1685,13 +1669,13 @@
         <v>24</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="K1" s="8" t="s">
         <v>7</v>
@@ -1712,16 +1696,16 @@
         <v>27</v>
       </c>
       <c r="Q1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="T1" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="U1" s="9" t="s">
         <v>9</v>
@@ -1736,42 +1720,42 @@
         <v>11</v>
       </c>
       <c r="Y1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="AA1" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB1" s="13" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="AC1" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AD1" s="13" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="AE1" s="13" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="AF1" s="13" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="AG1" s="13" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -1798,10 +1782,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="O2" s="1" t="b">
         <v>0</v>
@@ -1825,22 +1809,22 @@
         <v>2</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Z2" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AA2" s="1">
         <v>1</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AD2" s="1">
         <v>23960</v>
@@ -1860,7 +1844,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="X2">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1869,11 +1853,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E94CD2-F881-4057-99CD-CBE2B9D96557}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" activeCellId="1" sqref="H17 G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,10 +1899,10 @@
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>23</v>
@@ -1948,13 +1932,13 @@
         <v>8</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>28</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>9</v>
@@ -1969,24 +1953,24 @@
         <v>13</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="W1" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2013,7 +1997,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>0</v>
@@ -2031,13 +2015,13 @@
         <v>10</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
@@ -2057,10 +2041,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B4FA9B-1F49-4C23-93F7-CC7DAC82722D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
@@ -2107,10 +2091,10 @@
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>23</v>
@@ -2140,13 +2124,13 @@
         <v>8</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O1" s="10" t="s">
         <v>28</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="9" t="s">
         <v>9</v>
@@ -2161,40 +2145,40 @@
         <v>13</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="W1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="X1" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD1" s="16" t="s">
+      <c r="AF1" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF1" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="AG1" s="13" t="s">
         <v>17</v>
@@ -2211,13 +2195,13 @@
     </row>
     <row r="2" spans="1:36" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
@@ -2244,7 +2228,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>0</v>
@@ -2268,7 +2252,7 @@
         <v>5</v>
       </c>
       <c r="V2" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="W2" s="1">
         <v>1</v>
@@ -2413,18 +2397,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2446,14 +2430,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53ADD2F5-A402-45D1-88A3-5F6CA6334DE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2467,4 +2443,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40835504-4F46-4A81-BD00-C7B4354D2E50}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>